<commit_message>
Update public files from controller
</commit_message>
<xml_diff>
--- a/public/closed_days.xlsx
+++ b/public/closed_days.xlsx
@@ -20,17 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
+  <si>
+    <t xml:space="preserve">08.01.2025</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="d/mm/yyyy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -44,16 +48,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="238"/>
     </font>
     <font>
       <b val="true"/>
@@ -113,13 +120,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -314,10 +325,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -325,6 +336,11 @@
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>